<commit_message>
new dpeartment page is add and the some bug are fixed and systamise the code
</commit_message>
<xml_diff>
--- a/users.xlsx
+++ b/users.xlsx
@@ -5,13 +5,14 @@
   <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <sheets>
     <sheet sheetId="1" name="Users" state="visible" r:id="rId4"/>
+    <sheet sheetId="2" name="Sheet1" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
   <si>
     <t>Name</t>
   </si>
@@ -35,6 +36,36 @@
   </si>
   <si>
     <t>admin</t>
+  </si>
+  <si>
+    <t>manvir@gmail.com</t>
+  </si>
+  <si>
+    <t>$2b$10$L0t/oQGAv9yrvNydUZlEJ.82hG82dlVirYK5b6MC/AhuYhbRJPyNK</t>
+  </si>
+  <si>
+    <t>account</t>
+  </si>
+  <si>
+    <t>ujkhnm</t>
+  </si>
+  <si>
+    <t>a@gmail.com</t>
+  </si>
+  <si>
+    <t>$2b$10$dlbcjEB6WtCFJmI/oilfi.PNokRWWcn0EauwIRv1MPsv5dhdPzFbK</t>
+  </si>
+  <si>
+    <t>forensic</t>
+  </si>
+  <si>
+    <t>b@gmail.com</t>
+  </si>
+  <si>
+    <t>$2b$10$vxx.GROlTqWjBCFYhl3PJOP7g9HS0EjI1Mf0vf46Vmkqz3y4SZNjy</t>
+  </si>
+  <si>
+    <t>academics</t>
   </si>
 </sst>
 </file>
@@ -450,6 +481,73 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D4"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
bug of signup is solved
</commit_message>
<xml_diff>
--- a/users.xlsx
+++ b/users.xlsx
@@ -4,65 +4,55 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <sheets>
-    <sheet sheetId="1" name="Users" state="visible" r:id="rId4"/>
-    <sheet sheetId="2" name="Sheet1" state="visible" r:id="rId5"/>
+    <sheet sheetId="1" name="Sheet1" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Email</t>
-  </si>
-  <si>
-    <t>Password</t>
-  </si>
-  <si>
-    <t>Department</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>department</t>
   </si>
   <si>
     <t>manvir</t>
   </si>
   <si>
-    <t>manvi@gmil.com</t>
-  </si>
-  <si>
-    <t>$2b$10$UNJvIls0LQfL4I6JH4dz1eAfTt6PD3DAryyMhp51ozlGQPBfMGI6y</t>
-  </si>
-  <si>
-    <t>admin</t>
-  </si>
-  <si>
-    <t>manvir@gmail.com</t>
-  </si>
-  <si>
-    <t>$2b$10$L0t/oQGAv9yrvNydUZlEJ.82hG82dlVirYK5b6MC/AhuYhbRJPyNK</t>
-  </si>
-  <si>
-    <t>account</t>
-  </si>
-  <si>
-    <t>ujkhnm</t>
+    <t>g@gmail.com</t>
+  </si>
+  <si>
+    <t>$2b$10$wsiUzzuFg/VERhNRUvu72uJl.XTEiFH4P16D/cUxeBpYXIDz7ZkE6</t>
+  </si>
+  <si>
+    <t>forensic</t>
+  </si>
+  <si>
+    <t>manvir1</t>
+  </si>
+  <si>
+    <t>ga@gmail.com</t>
+  </si>
+  <si>
+    <t>$2b$10$LmUktpKzoDl3RXiWEnrxoOJU7zTotTiPqiljQk6gWz88p3e6ab2oG</t>
+  </si>
+  <si>
+    <t>mavnr</t>
   </si>
   <si>
     <t>a@gmail.com</t>
   </si>
   <si>
-    <t>$2b$10$dlbcjEB6WtCFJmI/oilfi.PNokRWWcn0EauwIRv1MPsv5dhdPzFbK</t>
-  </si>
-  <si>
-    <t>forensic</t>
-  </si>
-  <si>
-    <t>b@gmail.com</t>
-  </si>
-  <si>
-    <t>$2b$10$vxx.GROlTqWjBCFYhl3PJOP7g9HS0EjI1Mf0vf46Vmkqz3y4SZNjy</t>
+    <t>$2b$10$./0i/7lnt2iUMfH3hyRz8.8QOB.Yx/WYVNU5SNXtb709ZlXo8olFC</t>
   </si>
   <si>
     <t>academics</t>
@@ -442,51 +432,6 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
-  <cols>
-    <col min="1" max="1" width="20" customWidth="1"/>
-    <col min="2" max="2" width="30" customWidth="1"/>
-    <col min="3" max="3" width="40" customWidth="1"/>
-    <col min="4" max="4" width="20" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
@@ -509,41 +454,41 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>